<commit_message>
aggiunta 4 e 5 drupa 2021
</commit_message>
<xml_diff>
--- a/data-raw/2_Dati_monitoraggio.xlsx
+++ b/data-raw/2_Dati_monitoraggio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Desktop\file progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{141CD36C-0818-466B-A6C5-F6C6418CEABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9487EEE-53FD-455F-BE8D-5D836F5B42A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{771E8DDC-9830-4DB3-9034-8600F5654DC7}"/>
+    <workbookView xWindow="255" yWindow="120" windowWidth="25275" windowHeight="13755" xr2:uid="{771E8DDC-9830-4DB3-9034-8600F5654DC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="172">
   <si>
     <t>Codice_azienda</t>
   </si>
@@ -535,6 +535,21 @@
   </si>
   <si>
     <t>11_764-761</t>
+  </si>
+  <si>
+    <t>Clima</t>
+  </si>
+  <si>
+    <t>Mediterraneo_di_transizione</t>
+  </si>
+  <si>
+    <t>Temperato</t>
+  </si>
+  <si>
+    <t>Temperato_di_transizione</t>
+  </si>
+  <si>
+    <t>Mediterraneo</t>
   </si>
 </sst>
 </file>
@@ -886,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEAC1E44-BD4B-4A90-B572-0DDACD2085D7}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="L1" sqref="L1:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,9 +919,10 @@
     <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -940,8 +956,11 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -975,8 +994,11 @@
       <c r="K2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1010,8 +1032,11 @@
       <c r="K3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1045,8 +1070,11 @@
       <c r="K4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1080,8 +1108,11 @@
       <c r="K5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1115,8 +1146,11 @@
       <c r="K6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1150,8 +1184,11 @@
       <c r="K7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1185,8 +1222,11 @@
       <c r="K8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1220,8 +1260,11 @@
       <c r="K9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -1255,8 +1298,11 @@
       <c r="K10" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -1290,8 +1336,11 @@
       <c r="K11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -1325,8 +1374,11 @@
       <c r="K12" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>78</v>
       </c>
@@ -1360,8 +1412,11 @@
       <c r="K13" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -1395,8 +1450,11 @@
       <c r="K14" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -1430,8 +1488,11 @@
       <c r="K15" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -1465,8 +1526,11 @@
       <c r="K16" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -1500,8 +1564,11 @@
       <c r="K17" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>109</v>
       </c>
@@ -1535,8 +1602,11 @@
       <c r="K18" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -1570,8 +1640,11 @@
       <c r="K19" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>122</v>
       </c>
@@ -1605,8 +1678,11 @@
       <c r="K20" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>129</v>
       </c>
@@ -1640,8 +1716,11 @@
       <c r="K21" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>135</v>
       </c>
@@ -1675,8 +1754,11 @@
       <c r="K22" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>140</v>
       </c>
@@ -1710,8 +1792,11 @@
       <c r="K23" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>145</v>
       </c>
@@ -1745,8 +1830,11 @@
       <c r="K24" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>150</v>
       </c>
@@ -1780,8 +1868,11 @@
       <c r="K25" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>158</v>
       </c>
@@ -1815,8 +1906,11 @@
       <c r="K26" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>162</v>
       </c>
@@ -1849,6 +1943,9 @@
       </c>
       <c r="K27" t="s">
         <v>163</v>
+      </c>
+      <c r="L27" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>